<commit_message>
Add Zone of Interest to Excel and for pprint
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Nextcloud/lego_africa/Arbeit/06_Projekte/2024/LEGO Datenbank/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180FDA2-436C-CE4B-81DC-CEF6812414D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3351CD0-E44F-4F59-916D-DDDBB862DF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power BusInfo" sheetId="111" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power BusInfo'!$L$9:$Q$19</definedName>
-    <definedName name="businfo">'Power BusInfo'!$B$3:$J$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power BusInfo'!$M$9:$R$19</definedName>
+    <definedName name="businfo">'Power BusInfo'!$B$3:$K$16</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
     <definedName name="dsmprofiles">#REF!</definedName>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>[°]</t>
+  </si>
+  <si>
+    <t>[yes, no]</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ZoneOfInterest</t>
   </si>
 </sst>
 </file>
@@ -409,12 +421,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Link" xfId="8" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -736,30 +748,30 @@
   <sheetPr codeName="Tabelle9">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:Q19"/>
+  <dimension ref="B1:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" customWidth="1"/>
-    <col min="4" max="9" width="11.796875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="11.3984375" style="4"/>
+    <col min="4" max="10" width="11.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:18" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
@@ -781,19 +793,22 @@
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="5"/>
@@ -806,8 +821,9 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="6"/>
@@ -820,8 +836,9 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="2:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="2:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -843,19 +860,22 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -880,20 +900,23 @@
       <c r="I7" s="12">
         <v>0.95</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="2">
         <v>2000</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>2023</v>
       </c>
-      <c r="L7" s="13">
+      <c r="M7" s="13">
         <v>47.272599999999997</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>11.471399999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -918,18 +941,21 @@
       <c r="I8" s="12">
         <v>0.95</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="2">
         <v>2024</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="13">
+      <c r="L8" s="2"/>
+      <c r="M8" s="13">
         <v>47.233400000000003</v>
       </c>
-      <c r="M8" s="13">
+      <c r="N8" s="13">
         <v>11.898199999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -954,18 +980,21 @@
       <c r="I9" s="12">
         <v>0.95</v>
       </c>
-      <c r="L9" s="13">
+      <c r="J9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="13">
         <v>48.357199999999999</v>
       </c>
-      <c r="M9" s="13">
+      <c r="N9" s="13">
         <v>16.379300000000001</v>
       </c>
-      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="2:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -990,18 +1019,21 @@
       <c r="I10" s="12">
         <v>0.95</v>
       </c>
-      <c r="L10" s="13">
+      <c r="J10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="13">
         <v>48.181387999999998</v>
       </c>
-      <c r="M10" s="13">
+      <c r="N10" s="13">
         <v>16.433888</v>
       </c>
-      <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
@@ -1026,16 +1058,19 @@
       <c r="I11" s="12">
         <v>0.95</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="13">
+      <c r="L11" s="2"/>
+      <c r="M11" s="13">
         <v>48.122599999999998</v>
       </c>
-      <c r="M11" s="13">
+      <c r="N11" s="13">
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -1060,16 +1095,19 @@
       <c r="I12" s="12">
         <v>0.95</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="13">
+      <c r="L12" s="2"/>
+      <c r="M12" s="13">
         <v>48.032055</v>
       </c>
-      <c r="M12" s="13">
+      <c r="N12" s="13">
         <v>16.695450999999998</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
@@ -1094,16 +1132,19 @@
       <c r="I13" s="12">
         <v>0.95</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="13">
+      <c r="L13" s="2"/>
+      <c r="M13" s="13">
         <v>48.25749897</v>
       </c>
-      <c r="M13" s="13">
+      <c r="N13" s="13">
         <v>16.390085429999999</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
@@ -1128,16 +1169,19 @@
       <c r="I14" s="12">
         <v>0.95</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="13">
+      <c r="L14" s="2"/>
+      <c r="M14" s="13">
         <v>48.224722</v>
       </c>
-      <c r="M14" s="13">
+      <c r="N14" s="13">
         <v>15.689166</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1162,34 +1206,37 @@
       <c r="I15" s="12">
         <v>0.95</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="13">
+      <c r="L15" s="2"/>
+      <c r="M15" s="13">
         <v>48.1464</v>
       </c>
-      <c r="M15" s="13">
+      <c r="N15" s="13">
         <v>15.05</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="L16" s="2"/>
-      <c r="P16" s="14"/>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="M16" s="2"/>
       <c r="Q16" s="14"/>
-    </row>
-    <row r="17" spans="12:17" x14ac:dyDescent="0.2">
-      <c r="L17" s="2"/>
-      <c r="P17" s="14"/>
+      <c r="R16" s="14"/>
+    </row>
+    <row r="17" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M17" s="2"/>
       <c r="Q17" s="14"/>
-    </row>
-    <row r="18" spans="12:17" x14ac:dyDescent="0.2">
-      <c r="L18" s="2"/>
-      <c r="P18" s="14"/>
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M18" s="2"/>
       <c r="Q18" s="14"/>
-    </row>
-    <row r="19" spans="12:17" x14ac:dyDescent="0.2">
-      <c r="L19" s="2"/>
-      <c r="P19" s="14"/>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M19" s="2"/>
       <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1199,6 +1246,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1344,22 +1406,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1375,28 +1446,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set ExisUnits based on original LEGO optimization run
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3351CD0-E44F-4F59-916D-DDDBB862DF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A6EF07-BAE8-479C-8BEA-24D8571FC1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -751,7 +751,7 @@
   <dimension ref="B1:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1059,7 @@
         <v>0.95</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1096,7 +1096,7 @@
         <v>0.95</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>

</xml_diff>

<commit_message>
Mover get_dPower_Network to InOutModule
Fix Excl.-Column in Power_BusInfo
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE250D8F-0615-41C7-8B88-452DDB94A48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2842AA-75DF-4363-8577-AFA2FCB7EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -592,7 +592,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -637,9 +637,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1035,7 +1032,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1088,8 +1085,10 @@
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -1139,7 +1138,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
@@ -1190,7 +1189,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
         <v>61</v>
       </c>
@@ -1241,7 +1240,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
@@ -1292,12 +1291,12 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E8" s="12">
@@ -1309,40 +1308,40 @@
       <c r="G8" s="12">
         <v>0.9</v>
       </c>
-      <c r="H8" s="27">
-        <v>0</v>
-      </c>
-      <c r="I8" s="27">
-        <v>0</v>
-      </c>
-      <c r="J8" s="27">
+      <c r="H8" s="26">
+        <v>0</v>
+      </c>
+      <c r="I8" s="26">
+        <v>0</v>
+      </c>
+      <c r="J8" s="26">
         <v>0.95</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="21">
         <v>2000</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="21">
         <v>2023</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="27">
         <v>47.272599999999997</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="27">
         <v>11.471399999999999</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="21">
         <v>1</v>
       </c>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E9" s="12">
@@ -1354,40 +1353,40 @@
       <c r="G9" s="12">
         <v>0.9</v>
       </c>
-      <c r="H9" s="27">
-        <v>0</v>
-      </c>
-      <c r="I9" s="27">
-        <v>0</v>
-      </c>
-      <c r="J9" s="27">
+      <c r="H9" s="26">
+        <v>0</v>
+      </c>
+      <c r="I9" s="26">
+        <v>0</v>
+      </c>
+      <c r="J9" s="26">
         <v>0.95</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="21">
         <v>2024</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="28">
+      <c r="L9" s="21"/>
+      <c r="M9" s="27">
         <v>47.233400000000003</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="27">
         <v>11.898199999999999</v>
       </c>
-      <c r="O9" s="22">
+      <c r="O9" s="21">
         <v>1</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E10" s="12">
@@ -1399,38 +1398,38 @@
       <c r="G10" s="12">
         <v>0.9</v>
       </c>
-      <c r="H10" s="27">
-        <v>0</v>
-      </c>
-      <c r="I10" s="27">
-        <v>0</v>
-      </c>
-      <c r="J10" s="27">
+      <c r="H10" s="26">
+        <v>0</v>
+      </c>
+      <c r="I10" s="26">
+        <v>0</v>
+      </c>
+      <c r="J10" s="26">
         <v>0.95</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="28">
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="27">
         <v>48.357199999999999</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="27">
         <v>16.379300000000001</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="21">
         <v>1</v>
       </c>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E11" s="12">
@@ -1442,36 +1441,36 @@
       <c r="G11" s="12">
         <v>0.9</v>
       </c>
-      <c r="H11" s="27">
-        <v>0</v>
-      </c>
-      <c r="I11" s="27">
-        <v>0</v>
-      </c>
-      <c r="J11" s="27">
+      <c r="H11" s="26">
+        <v>0</v>
+      </c>
+      <c r="I11" s="26">
+        <v>0</v>
+      </c>
+      <c r="J11" s="26">
         <v>0.95</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="28">
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="27">
         <v>48.181387999999998</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="27">
         <v>16.433888</v>
       </c>
-      <c r="O11" s="22">
-        <v>0</v>
-      </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
+      <c r="O11" s="21">
+        <v>0</v>
+      </c>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E12" s="12">
@@ -1483,36 +1482,36 @@
       <c r="G12" s="12">
         <v>0.9</v>
       </c>
-      <c r="H12" s="27">
-        <v>0</v>
-      </c>
-      <c r="I12" s="27">
-        <v>0</v>
-      </c>
-      <c r="J12" s="27">
+      <c r="H12" s="26">
+        <v>0</v>
+      </c>
+      <c r="I12" s="26">
+        <v>0</v>
+      </c>
+      <c r="J12" s="26">
         <v>0.95</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="28">
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="27">
         <v>48.122599999999998</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="27">
         <v>16.420000000000002</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="21">
         <v>1</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E13" s="12">
@@ -1524,36 +1523,36 @@
       <c r="G13" s="12">
         <v>0.9</v>
       </c>
-      <c r="H13" s="27">
-        <v>0</v>
-      </c>
-      <c r="I13" s="27">
-        <v>0</v>
-      </c>
-      <c r="J13" s="27">
+      <c r="H13" s="26">
+        <v>0</v>
+      </c>
+      <c r="I13" s="26">
+        <v>0</v>
+      </c>
+      <c r="J13" s="26">
         <v>0.95</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="28">
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="27">
         <v>48.032055</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="27">
         <v>16.695450999999998</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="21">
         <v>1</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="12">
@@ -1565,36 +1564,36 @@
       <c r="G14" s="12">
         <v>0.9</v>
       </c>
-      <c r="H14" s="27">
-        <v>0</v>
-      </c>
-      <c r="I14" s="27">
-        <v>0</v>
-      </c>
-      <c r="J14" s="27">
+      <c r="H14" s="26">
+        <v>0</v>
+      </c>
+      <c r="I14" s="26">
+        <v>0</v>
+      </c>
+      <c r="J14" s="26">
         <v>0.95</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="28">
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="27">
         <v>48.25749897</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="27">
         <v>16.390085429999999</v>
       </c>
-      <c r="O14" s="22">
-        <v>0</v>
-      </c>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="12">
@@ -1606,36 +1605,36 @@
       <c r="G15" s="12">
         <v>0.9</v>
       </c>
-      <c r="H15" s="27">
-        <v>0</v>
-      </c>
-      <c r="I15" s="27">
-        <v>0</v>
-      </c>
-      <c r="J15" s="27">
+      <c r="H15" s="26">
+        <v>0</v>
+      </c>
+      <c r="I15" s="26">
+        <v>0</v>
+      </c>
+      <c r="J15" s="26">
         <v>0.95</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="28">
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="27">
         <v>48.224722</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="27">
         <v>15.689166</v>
       </c>
-      <c r="O15" s="22">
-        <v>0</v>
-      </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="30"/>
+      <c r="O15" s="21">
+        <v>0</v>
+      </c>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="29"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="12">
@@ -1647,28 +1646,28 @@
       <c r="G16" s="12">
         <v>0.9</v>
       </c>
-      <c r="H16" s="27">
-        <v>0</v>
-      </c>
-      <c r="I16" s="27">
-        <v>0</v>
-      </c>
-      <c r="J16" s="27">
+      <c r="H16" s="26">
+        <v>0</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0</v>
+      </c>
+      <c r="J16" s="26">
         <v>0.95</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="28">
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="27">
         <v>48.1464</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="27">
         <v>15.05</v>
       </c>
-      <c r="O16" s="22">
-        <v>0</v>
-      </c>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="30"/>
+      <c r="O16" s="21">
+        <v>0</v>
+      </c>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="29"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
@@ -1680,12 +1679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1831,6 +1824,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1841,22 +1840,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1874,6 +1857,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adjust Power_BusInfo to v0.0.3r
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2842AA-75DF-4363-8577-AFA2FCB7EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E19C71-FA23-49AA-AE80-C7DFCAA85313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>pBusB</t>
   </si>
   <si>
-    <t>Suceptance B connected to node</t>
-  </si>
-  <si>
     <t>Conductance G connected to node</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>Year where it is decommissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>[0, 1]</t>
   </si>
   <si>
@@ -376,6 +370,12 @@
   </si>
   <si>
     <t>StylizedSystem</t>
+  </si>
+  <si>
+    <t>Susceptance B connected to node</t>
+  </si>
+  <si>
+    <t>v0.0.3r</t>
   </si>
 </sst>
 </file>
@@ -1025,15 +1025,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1060,33 +1060,33 @@
         <v>2</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -1110,31 +1110,31 @@
         <v>35</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1158,97 +1158,97 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="M5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -1281,13 +1281,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -1342,7 +1342,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -1387,7 +1387,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -1430,7 +1430,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -1471,7 +1471,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -1512,7 +1512,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -1553,7 +1553,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -1594,7 +1594,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -1635,7 +1635,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -1679,6 +1679,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1824,35 +1839,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1874,9 +1864,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust Power_BusInfo to v0.0.4r
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E19C71-FA23-49AA-AE80-C7DFCAA85313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E14A04-869F-421B-82FD-98790EAE036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -297,12 +297,6 @@
     <t>Decommission Year</t>
   </si>
   <si>
-    <t>comYear</t>
-  </si>
-  <si>
-    <t>decomYear</t>
-  </si>
-  <si>
     <t>[db-key]</t>
   </si>
   <si>
@@ -375,7 +369,16 @@
     <t>Susceptance B connected to node</t>
   </si>
   <si>
-    <t>v0.0.3r</t>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>YearCom</t>
+  </si>
+  <si>
+    <t>YearDecom</t>
   </si>
 </sst>
 </file>
@@ -1025,15 +1028,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1075,18 +1078,18 @@
         <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="Q3" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>64</v>
+      <c r="A4" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -1115,11 +1118,11 @@
       <c r="J4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>47</v>
+      <c r="K4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
@@ -1128,13 +1131,13 @@
         <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="Q4" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1158,7 +1161,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>36</v>
@@ -1167,10 +1170,10 @@
         <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>42</v>
@@ -1179,76 +1182,76 @@
         <v>43</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>62</v>
-      </c>
       <c r="L6" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -1281,13 +1284,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1297,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -1342,7 +1345,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -1387,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -1430,7 +1433,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -1471,7 +1474,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -1512,7 +1515,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -1553,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -1594,7 +1597,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -1635,7 +1638,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -1679,18 +1682,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1840,14 +1843,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1859,6 +1854,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adjust scenario names in Power_BusInfo & Power_Network
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E14A04-869F-421B-82FD-98790EAE036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD963E-F06B-4281-B8F7-C49F027F3505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="111" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarioA!$L$9:$S$16</definedName>
-    <definedName name="businfo">scenarioA!$B$3:$O$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScenarioA!$L$9:$S$16</definedName>
+    <definedName name="businfo">ScenarioA!$B$3:$O$16</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
     <definedName name="dsmprofiles">#REF!</definedName>
@@ -1072,10 +1072,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>49</v>
@@ -1682,21 +1682,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1842,31 +1827,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1882,4 +1858,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix pyomo vLineP, vLineQ, vGenQ handeling. Add bounds for quadratic variables
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD963E-F06B-4281-B8F7-C49F027F3505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFD4837-B9AB-4137-8529-9BF1BAD76076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72850" yWindow="2170" windowWidth="38620" windowHeight="21100" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="111" r:id="rId1"/>
@@ -678,11 +678,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -1010,23 +1010,23 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.1328125" style="3" customWidth="1"/>
     <col min="2" max="16" width="20" style="3" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="3"/>
+    <col min="17" max="17" width="24.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B2" s="16" t="s">
         <v>61</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="25" t="s">
         <v>62</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="18" t="s">
         <v>71</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="8" customFormat="1" ht="43" x14ac:dyDescent="0.45">
       <c r="A5" s="19"/>
       <c r="B5" s="9" t="s">
         <v>29</v>
@@ -1191,7 +1191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="8" customFormat="1" ht="43" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
         <v>58</v>
@@ -1242,7 +1242,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>46</v>
@@ -1293,7 +1293,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" s="28"/>
       <c r="B8" s="22"/>
       <c r="C8" s="23" t="s">
@@ -1312,10 +1312,10 @@
         <v>0.9</v>
       </c>
       <c r="H8" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="26">
         <v>0.95</v>
@@ -1338,7 +1338,7 @@
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="28"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23" t="s">
@@ -1357,10 +1357,10 @@
         <v>0.9</v>
       </c>
       <c r="H9" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="26">
         <v>0.95</v>
@@ -1383,7 +1383,7 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="28"/>
       <c r="B10" s="22"/>
       <c r="C10" s="23" t="s">
@@ -1402,10 +1402,10 @@
         <v>0.9</v>
       </c>
       <c r="H10" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="26">
         <v>0.95</v>
@@ -1426,7 +1426,7 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="28"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23" t="s">
@@ -1445,10 +1445,10 @@
         <v>0.9</v>
       </c>
       <c r="H11" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="26">
         <v>0.95</v>
@@ -1467,7 +1467,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" s="28"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23" t="s">
@@ -1486,10 +1486,10 @@
         <v>0.9</v>
       </c>
       <c r="H12" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="26">
         <v>0.95</v>
@@ -1508,7 +1508,7 @@
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" s="28"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
@@ -1527,10 +1527,10 @@
         <v>0.9</v>
       </c>
       <c r="H13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="26">
         <v>0.95</v>
@@ -1549,7 +1549,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" s="28"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23" t="s">
@@ -1568,10 +1568,10 @@
         <v>0.9</v>
       </c>
       <c r="H14" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="26">
         <v>0.95</v>
@@ -1590,7 +1590,7 @@
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" s="28"/>
       <c r="B15" s="22"/>
       <c r="C15" s="23" t="s">
@@ -1609,10 +1609,10 @@
         <v>0.9</v>
       </c>
       <c r="H15" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="26">
         <v>0.95</v>
@@ -1631,7 +1631,7 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="29"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" s="28"/>
       <c r="B16" s="22"/>
       <c r="C16" s="23" t="s">
@@ -1650,10 +1650,10 @@
         <v>0.9</v>
       </c>
       <c r="H16" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="26">
         <v>0.95</v>
@@ -1682,6 +1682,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1827,15 +1836,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1843,6 +1843,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1856,14 +1864,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix SOCP constraint handling
</commit_message>
<xml_diff>
--- a/data/example/Power_BusInfo.xlsx
+++ b/data/example/Power_BusInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFD4837-B9AB-4137-8529-9BF1BAD76076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573D7250-5215-44EF-8406-9DB903C400AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72850" yWindow="2170" windowWidth="38620" windowHeight="21100" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="79260" yWindow="7730" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="111" r:id="rId1"/>
@@ -1010,7 +1010,7 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1312,10 +1312,10 @@
         <v>0.9</v>
       </c>
       <c r="H8" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="26">
         <v>0.95</v>
@@ -1357,10 +1357,10 @@
         <v>0.9</v>
       </c>
       <c r="H9" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="26">
         <v>0.95</v>
@@ -1402,10 +1402,10 @@
         <v>0.9</v>
       </c>
       <c r="H10" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="26">
         <v>0.95</v>
@@ -1445,10 +1445,10 @@
         <v>0.9</v>
       </c>
       <c r="H11" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="26">
         <v>0.95</v>
@@ -1486,10 +1486,10 @@
         <v>0.9</v>
       </c>
       <c r="H12" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="26">
         <v>0.95</v>
@@ -1527,10 +1527,10 @@
         <v>0.9</v>
       </c>
       <c r="H13" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="26">
         <v>0.95</v>
@@ -1568,10 +1568,10 @@
         <v>0.9</v>
       </c>
       <c r="H14" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="26">
         <v>0.95</v>
@@ -1609,10 +1609,10 @@
         <v>0.9</v>
       </c>
       <c r="H15" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="26">
         <v>0.95</v>
@@ -1650,10 +1650,10 @@
         <v>0.9</v>
       </c>
       <c r="H16" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="26">
         <v>0.95</v>
@@ -1682,12 +1682,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1837,15 +1834,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1869,17 +1877,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>